<commit_message>
feat:update obby new level
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Obbycheck_检查点表.xlsx
+++ b/dragon-verse/Excels/Obbycheck_检查点表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>int</t>
   </si>
@@ -237,6 +237,36 @@
   </si>
   <si>
     <t>390054.81|8562.91|30876.23</t>
+  </si>
+  <si>
+    <t>393397.53|8672.15|31400.97</t>
+  </si>
+  <si>
+    <t>393400.94|8666.14|31052.23</t>
+  </si>
+  <si>
+    <t>396374.53|8289.15|31400.97</t>
+  </si>
+  <si>
+    <t>396378.94|8299.14|31052.23</t>
+  </si>
+  <si>
+    <t>394144.53|7755.15|31599.97</t>
+  </si>
+  <si>
+    <t>394154.94|7762.14|31500.23</t>
+  </si>
+  <si>
+    <t>396558.53|8610.15|32502.97</t>
+  </si>
+  <si>
+    <t>396563.94|8594.14|32177.23</t>
+  </si>
+  <si>
+    <t>399253.53|8610.15|33974.97</t>
+  </si>
+  <si>
+    <t>399263.94|8611.14|33564.23</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1222,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -1667,6 +1697,76 @@
         <v>11</v>
       </c>
     </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>